<commit_message>
Change error on uncentralized data to #VALUE!
</commit_message>
<xml_diff>
--- a/Demo.xlsx
+++ b/Demo.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\Desktop\LambdaPCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LambdaPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A74AFA-99C6-47F2-89DE-42FF6816C9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B074467-ECDB-4A86-9C73-B0C61EF211AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="18920" windowHeight="8560" xr2:uid="{61C23DE5-AA8F-4447-8136-F74E018A438C}"/>
+    <workbookView xWindow="280" yWindow="20" windowWidth="18920" windowHeight="8560" xr2:uid="{61C23DE5-AA8F-4447-8136-F74E018A438C}"/>
   </bookViews>
   <sheets>
     <sheet name="IrisPCA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="PCA">_xlfn.LAMBDA(_xlpm.array,_xlpm.tolerance,_xlpm.centralityCheck,_xlfn.LET(_xlpm.tolerance_,IF(_xlfn.ISOMITTED(_xlpm.tolerance),0.0000001,_xlpm.tolerance),_xlpm.cCheck_,IF(_xlfn.ISOMITTED(_xlpm.centralityCheck),0.0000001,_xlpm.centralityCheck),_xlpm.worstAvg,MAX(_xlfn.BYCOL(_xlpm.array,_xlfn.LAMBDA(_xlpm.col,AVERAGE(_xlpm.col)))),IF(AND(TYPE(_xlpm.cCheck_)=1,_xlpm.cCheck_&gt;=0,_xlpm.worstAvg&gt;=_xlpm.cCheck_),"The input to PCA must be centralized. That is, the mean of each column must be close to zero",_xlfn.LET(_xlpm.nCols,COLUMNS(_xlpm.array),_xlpm.covMatrix,_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.iRow,_xlpm.iCol,_xlfn.COVARIANCE.P(INDEX(_xlpm.array,0,_xlpm.iRow),INDEX(_xlpm.array,0,_xlpm.iCol)))),_xlpm.system,_xlfn.VSTACK(_xlpm.covMatrix,_xlfn.MUNIT(COLUMNS(_xlpm.covMatrix))),_xlpm.fullResult,PCA_INTERNAL(_xlpm.system,_xlpm.tolerance_),_xlpm.varVector,INDEX(_xlpm.fullResult,_xlfn.SEQUENCE(_xlpm.nCols),_xlfn.SEQUENCE(_xlpm.nCols)),_xlpm.idx,_xlfn.SORTBY(_xlfn.SEQUENCE(_xlpm.nCols),_xlpm.varVector,-1),_xlpm.uncoeffs,INDEX(_xlpm.fullResult,_xlfn.SEQUENCE(_xlpm.nCols,1,_xlpm.nCols+1),_xlfn.SEQUENCE(1,_xlpm.nCols)),_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.iRow,_xlpm.iCol,INDEX(_xlpm.uncoeffs,INDEX(_xlpm.idx,_xlpm.iRow,1),_xlpm.iCol)))))))</definedName>
+    <definedName name="PCA">_xlfn.LAMBDA(_xlpm.array,_xlpm.tolerance,_xlpm.centralityCheck,_xlfn.LET(_xlpm.tolerance_,IF(_xlfn.ISOMITTED(_xlpm.tolerance),0.0000001,_xlpm.tolerance),_xlpm.cCheck_,IF(_xlfn.ISOMITTED(_xlpm.centralityCheck),0.0000001,_xlpm.centralityCheck),_xlpm.worstAvg,MAX(_xlfn.BYCOL(_xlpm.array,_xlfn.LAMBDA(_xlpm.col,AVERAGE(_xlpm.col)))),IF(AND(TYPE(_xlpm.cCheck_)=1,_xlpm.cCheck_&gt;=0,_xlpm.worstAvg&gt;=_xlpm.cCheck_),(--""),_xlfn.LET(_xlpm.nCols,COLUMNS(_xlpm.array),_xlpm.covMatrix,_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.iRow,_xlpm.iCol,_xlfn.COVARIANCE.P(INDEX(_xlpm.array,0,_xlpm.iRow),INDEX(_xlpm.array,0,_xlpm.iCol)))),_xlpm.system,_xlfn.VSTACK(_xlpm.covMatrix,_xlfn.MUNIT(COLUMNS(_xlpm.covMatrix))),_xlpm.fullResult,PCA_INTERNAL(_xlpm.system,_xlpm.tolerance_),_xlpm.varVector,INDEX(_xlpm.fullResult,_xlfn.SEQUENCE(_xlpm.nCols),_xlfn.SEQUENCE(_xlpm.nCols)),_xlpm.idx,_xlfn.SORTBY(_xlfn.SEQUENCE(_xlpm.nCols),_xlpm.varVector,-1),_xlpm.uncoeffs,INDEX(_xlpm.fullResult,_xlfn.SEQUENCE(_xlpm.nCols,1,_xlpm.nCols+1),_xlfn.SEQUENCE(1,_xlpm.nCols)),_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.iRow,_xlpm.iCol,INDEX(_xlpm.uncoeffs,INDEX(_xlpm.idx,_xlpm.iRow,1),_xlpm.iCol)))))))</definedName>
     <definedName name="PCA_INTERNAL">_xlfn.LAMBDA(_xlpm.system,_xlpm.tolerance,_xlfn.LET(_xlpm.nCols,COLUMNS(_xlpm.system),_xlpm.covMatrix,INDEX(_xlpm.system,_xlfn.SEQUENCE(_xlpm.nCols),_xlfn.SEQUENCE(1,_xlpm.nCols)),_xlpm.accJacobi,INDEX(_xlpm.system,_xlfn.SEQUENCE(_xlpm.nCols,1,_xlpm.nCols+1),_xlfn.SEQUENCE(1,_xlpm.nCols)),_xlpm.covLower,_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.iRow,_xlpm.iCol,IF(_xlpm.iCol&gt;_xlpm.iRow-1,0,INDEX(_xlpm.covMatrix,_xlpm.iRow,_xlpm.iCol)))),_xlpm.covAbs,ABS(_xlpm.covLower),_xlpm.worst,MAX(_xlpm.covAbs),IF(_xlpm.worst&lt;_xlpm.tolerance,_xlpm.system,_xlfn.LET(_xlpm.worstInRow,_xlfn.BYROW(_xlpm.covAbs,_xlfn.LAMBDA(_xlpm.x,MAX(_xlpm.x))),_xlpm.wRow,MATCH(_xlpm.worst,_xlpm.worstInRow,0),_xlpm.worstInCol,_xlfn.BYCOL(_xlpm.covAbs,_xlfn.LAMBDA(_xlpm.x,MAX(_xlpm.x))),_xlpm.wCol,MATCH(_xlpm.worst,_xlpm.worstInCol,0),_xlpm.tau,(INDEX(_xlpm.covMatrix,_xlpm.wRow,_xlpm.wRow)-INDEX(_xlpm.covMatrix,_xlpm.wCol,_xlpm.wCol))/(2*INDEX(_xlpm.covMatrix,_xlpm.wRow,_xlpm.wCol)),_xlpm.t_,IF(_xlpm.tau&lt;0,-_xlpm.tau-SQRT(1+_xlpm.tau*_xlpm.tau),-_xlpm.tau+SQRT(1+_xlpm.tau*_xlpm.tau)),_xlpm.cval,1/SQRT(1+_xlpm.t_*_xlpm.t_),_xlpm.sval,_xlpm.cval*_xlpm.t_,_xlpm.jacobi,_xlfn.MAKEARRAY(_xlpm.nCols,_xlpm.nCols,_xlfn.LAMBDA(_xlpm.jRow,_xlpm.jCol,IF(AND(_xlpm.jRow=_xlpm.wCol,_xlpm.jCol=_xlpm.wCol),_xlpm.cval,IF(AND(_xlpm.jRow=_xlpm.wRow,_xlpm.jCol=_xlpm.wRow),_xlpm.cval,IF(AND(_xlpm.jRow=_xlpm.wCol,_xlpm.jCol=_xlpm.wRow),_xlpm.sval,IF(AND(_xlpm.jRow=_xlpm.wRow,_xlpm.jCol=_xlpm.wCol),-_xlpm.sval,IF(AND(_xlpm.jRow=_xlpm.jCol),1,0))))))),_xlpm.newCovMatrix,MMULT(MMULT(TRANSPOSE(_xlpm.jacobi),_xlpm.covMatrix),_xlpm.jacobi),_xlpm.newAccJacobi,MMULT(TRANSPOSE(_xlpm.jacobi),_xlpm.accJacobi),PCA_INTERNAL(_xlfn.VSTACK(_xlpm.newCovMatrix,_xlpm.newAccJacobi),_xlpm.tolerance)))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -111,8 +111,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -165,7 +165,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -173,7 +173,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,15 +579,15 @@
         <v>-0.74333333333333496</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G66" si="0">B3-AVERAGE(B$3:B$152)</f>
+        <f t="shared" ref="G3" si="0">B3-AVERAGE(B$3:B$152)</f>
         <v>0.44599999999999929</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H66" si="1">C3-AVERAGE(C$3:C$152)</f>
+        <f t="shared" ref="H3" si="1">C3-AVERAGE(C$3:C$152)</f>
         <v>-2.3586666666666694</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I66" si="2">D3-AVERAGE(D$3:D$152)</f>
+        <f t="shared" ref="I3" si="2">D3-AVERAGE(D$3:D$152)</f>
         <v>-0.99866666666666726</v>
       </c>
       <c r="K3" s="1" cm="1">

</xml_diff>